<commit_message>
add the calculation for F2017068
</commit_message>
<xml_diff>
--- a/lotteries/zone.xlsx
+++ b/lotteries/zone.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="10350"/>
+    <workbookView windowWidth="23895" windowHeight="10350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="D" sheetId="1" r:id="rId1"/>
@@ -17,15 +17,38 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -46,11 +69,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -78,48 +128,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -138,14 +146,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,6 +196,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -220,6 +232,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -250,30 +280,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -286,6 +292,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -299,66 +359,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,6 +381,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -417,41 +447,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,10 +489,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -501,133 +501,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -963,8 +963,8 @@
   <sheetPr/>
   <dimension ref="A1:AI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.75833333333333" defaultRowHeight="13.5"/>
@@ -1174,10 +1174,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AG11"/>
+  <dimension ref="A1:AG13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG1" sqref="I1:AG35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.00833333333333" defaultRowHeight="13.5"/>
@@ -1286,85 +1286,101 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="2:21">
-      <c r="B2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="H2" s="1"/>
+    <row r="2" spans="1:29">
+      <c r="A2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="2:28">
-      <c r="B3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="12:31">
+      <c r="R2" s="1"/>
+      <c r="AC2" s="1"/>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="2:21">
+      <c r="B4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="AE4" s="1"/>
-    </row>
-    <row r="5" spans="1:31">
-      <c r="A5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="2:28">
+      <c r="B5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="P5" s="1"/>
       <c r="V5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AE5" s="1"/>
-    </row>
-    <row r="6" spans="6:27">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="12:31">
       <c r="L6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-    </row>
-    <row r="7" spans="5:31">
-      <c r="E7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="AE6" s="1"/>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="V7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="4:25">
-      <c r="D8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="Y8" s="1"/>
-    </row>
-    <row r="9" spans="1:32">
-      <c r="A9" s="1"/>
-      <c r="I9" s="1"/>
+    <row r="8" spans="6:27">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+    </row>
+    <row r="9" spans="5:31">
+      <c r="E9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AF9" s="1"/>
-    </row>
-    <row r="10" spans="18:31">
-      <c r="R10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-    </row>
-    <row r="11" spans="13:28">
+      <c r="X9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AE9" s="1"/>
+    </row>
+    <row r="10" spans="4:25">
+      <c r="D10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="Y10" s="1"/>
+    </row>
+    <row r="11" spans="1:32">
+      <c r="A11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
       <c r="AB11" s="1"/>
+      <c r="AF11" s="1"/>
+    </row>
+    <row r="12" spans="18:31">
+      <c r="R12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+    </row>
+    <row r="13" spans="13:28">
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="AB13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>